<commit_message>
2 issues solved 08/04/2025
</commit_message>
<xml_diff>
--- a/templates/Excel/ST1_Line_Setup.xlsx
+++ b/templates/Excel/ST1_Line_Setup.xlsx
@@ -563,32 +563,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-03-26T12:33</t>
+          <t>2025-04-03T15:03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SHIFT_1</t>
+          <t>SHIFT_2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.3</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -623,42 +623,42 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>1.23</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>2.63</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>32.3</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -673,17 +673,17 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Suriya</t>
+          <t>o</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>Suriya</t>
+          <t>o</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>Suriya</t>
+          <t>o</t>
         </is>
       </c>
     </row>

</xml_diff>